<commit_message>
Renamed count table directory.
Changed the sample sheet to have the more desirable naming scheme and
renamed the count tables accordingly.
</commit_message>
<xml_diff>
--- a/sample_sheets/all_samples.xlsx
+++ b/sample_sheets/all_samples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="143">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -119,7 +119,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0564/hpgl0564_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0564/hpgl0564_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0564/hpgl0564_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0565</t>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0565/hpgl0565_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0565/hpgl0565_scerevisiae.count.xz</t>
+    <t xml:space="preserve">Preprocessing/E1/hpgl0565/hpgl0565_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0566</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0566/hpgl0566_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0566/hpgl0566_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0566/hpgl0566_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0567</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0567/hpgl0567_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0567/hpgl0567_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0567/hpgl0567_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0568</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0568/hpgl0568_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0568/hpgl0568_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0568/hpgl0568_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0569</t>
@@ -188,7 +188,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0569/hpgl0569_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0569/hpgl0569_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0569/hpgl0569_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0570</t>
@@ -200,7 +200,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0570/hpgl0570_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0570/hpgl0570_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0570/hpgl0570_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0571</t>
@@ -209,34 +209,115 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0571/hpgl0571_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v1/hpgl0571/hpgl0571_scerevisiae.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">processed_data/count_tables/wt/wt_forward-trimmed_scerevisiae.count.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upf1</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0571/hpgl0571_scerevisiae.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/v2/hpgl0774/outputs/bowtie2_scerevisiae/hpgl0774_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0774/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0774/outputs/bowtie2_scerevisiae/hpgl0774_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/v2/hpgl0775/outputs/bowtie2_scerevisiae/hpgl0775_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0775/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0775/outputs/bowtie2_scerevisiae/hpgl0775_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yJD1745</t>
   </si>
   <si>
     <t xml:space="preserve">upf1d</t>
   </si>
   <si>
-    <t xml:space="preserve">processed_data/count_tables/upf1/upf1_forward-trimmed_scerevisiae.count.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upf2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">processed_data/count_tables/upf2/upf2_forward-trimmed_scerevisiae.count.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upf3</t>
+    <t xml:space="preserve">wt ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 upf1::LEU2 + CBF5 on pRS313 (yJD1524 upf1Δ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/v2/hpgl0776/outputs/bowtie2_scerevisiae/hpgl0776_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0776/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0776/outputs/bowtie2_scerevisiae/hpgl0776_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yJD1746</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbf5_D95A upf1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d95a ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 upf1::LEU2 + CBF5 D95A on pRS313 (yJD1525 upf1Δ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/v2/hpgl0777/outputs/bowtie2_scerevisiae/hpgl0777_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0777/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0777/outputs/bowtie2_scerevisiae/hpgl0777_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/v2/hpgl0778/outputs/bowtie2_scerevisiae/hpgl0778_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0778/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0778/outputs/bowtie2_scerevisiae/hpgl0778_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/v2/hpgl0779/outputs/bowtie2_scerevisiae/hpgl0779_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0779/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0779/outputs/bowtie2_scerevisiae/hpgl0779_forward-trimmed.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpgl0780</t>
   </si>
   <si>
     <r>
@@ -261,100 +342,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">processed_data/count_tables/upf3/upf3_forward-trimmed_scereviaiae.count.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E2B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0774/outputs/bowtie2_scerevisiae/hpgl0774_forward-trimmed.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0774/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0775</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0775/outputs/bowtie2_scerevisiae/hpgl0775_forward-trimmed.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0775/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0776</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yJD1745</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wt ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 upf1::LEU2 + CBF5 on pRS313 (yJD1524 upf1Δ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0776/outputs/bowtie2_scerevisiae/hpgl0776_forward-trimmed.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0776/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yJD1746</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cbf5_D95A upf1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d95a ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 upf1::LEU2 + CBF5 D95A on pRS313 (yJD1525 upf1Δ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0777/outputs/bowtie2_scerevisiae/hpgl0777_forward-trimmed.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0777/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0778</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E2B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0778/outputs/bowtie2_scerevisiae/hpgl0778_forward-trimmed.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0778/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0779/outputs/bowtie2_scerevisiae/hpgl0779_forward-trimmed.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0779/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hpgl0780</t>
-  </si>
-  <si>
     <t xml:space="preserve">preprocessing/v2/hpgl0780/outputs/bowtie2_scerevisiae/hpgl0780_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0780/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0780/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0780/outputs/bowtie2_scerevisiae/hpgl0780_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0781</t>
@@ -363,7 +357,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0781/outputs/bowtie2_scerevisiae/hpgl0781_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0781/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0781/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0781/outputs/bowtie2_scerevisiae/hpgl0781_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0782</t>
@@ -378,7 +375,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0782/outputs/bowtie2_scerevisiae/hpgl0782_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0782/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0782/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0782/outputs/bowtie2_scerevisiae/hpgl0782_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0783</t>
@@ -390,7 +390,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0783/outputs/bowtie2_scerevisiae/hpgl0783_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0783/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0783/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0783/outputs/bowtie2_scerevisiae/hpgl0783_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0784</t>
@@ -399,7 +402,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0784/outputs/bowtie2_scerevisiae/hpgl0784_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0784/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0784/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0784/outputs/bowtie2_scerevisiae/hpgl0784_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0785</t>
@@ -408,7 +414,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0785/outputs/bowtie2_scerevisiae/hpgl0785_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0785/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0785/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0785/outputs/bowtie2_scerevisiae/hpgl0785_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0786</t>
@@ -423,7 +432,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0786/outputs/bowtie2_scerevisiae/hpgl0786_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0786/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0786/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0786/outputs/bowtie2_scerevisiae/hpgl0786_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0787</t>
@@ -432,7 +444,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0787/outputs/bowtie2_scerevisiae/hpgl0787_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0787/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0787/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0787/outputs/bowtie2_scerevisiae/hpgl0787_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0788</t>
@@ -441,7 +456,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0788/outputs/bowtie2_scerevisiae/hpgl0788_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0788/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0788/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0788/outputs/bowtie2_scerevisiae/hpgl0788_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0789</t>
@@ -450,7 +468,10 @@
     <t xml:space="preserve">preprocessing/v2/hpgl0789/outputs/bowtie2_scerevisiae/hpgl0789_forward-trimmed.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0789/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0789/outputs/bowtie2_scerevisiae/introns.count.xz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprocessing/E2/hpgl0789/outputs/bowtie2_scerevisiae/hpgl0789_forward-trimmed.count.xz</t>
   </si>
 </sst>
 </file>
@@ -492,15 +513,15 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Sans"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -559,7 +580,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,10 +601,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ32"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R28" activeCellId="0" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1098,153 +1119,185 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="Q13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AMJ13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="J14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="O14" s="3"/>
+      <c r="Q14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="O15" s="3"/>
+      <c r="Q15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AMJ15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AMJ16" s="0"/>
+        <v>65</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="3"/>
+      <c r="Q16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
@@ -1253,13 +1306,13 @@
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>27</v>
@@ -1268,25 +1321,25 @@
         <v>27</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="3"/>
       <c r="Q17" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>45</v>
@@ -1295,13 +1348,13 @@
         <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>47</v>
@@ -1310,7 +1363,7 @@
         <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>48</v>
@@ -1318,33 +1371,33 @@
       <c r="K18" s="2"/>
       <c r="O18" s="3"/>
       <c r="Q18" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
@@ -1353,44 +1406,44 @@
         <v>47</v>
       </c>
       <c r="I19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="O19" s="3"/>
       <c r="Q19" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="G20" s="1" t="s">
         <v>47</v>
       </c>
@@ -1398,10 +1451,10 @@
         <v>47</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1409,18 +1462,18 @@
       <c r="N20" s="2"/>
       <c r="O20" s="3"/>
       <c r="Q20" s="1" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
@@ -1429,13 +1482,13 @@
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>27</v>
@@ -1444,25 +1497,25 @@
         <v>27</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="3"/>
       <c r="Q21" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>45</v>
@@ -1471,13 +1524,13 @@
         <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>47</v>
@@ -1486,7 +1539,7 @@
         <v>27</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>48</v>
@@ -1494,33 +1547,33 @@
       <c r="K22" s="2"/>
       <c r="O22" s="3"/>
       <c r="Q22" s="1" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>27</v>
@@ -1529,43 +1582,43 @@
         <v>47</v>
       </c>
       <c r="I23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="O23" s="3"/>
       <c r="Q23" s="1" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>47</v>
@@ -1574,10 +1627,10 @@
         <v>47</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -1585,18 +1638,18 @@
       <c r="N24" s="2"/>
       <c r="O24" s="3"/>
       <c r="Q24" s="1" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
@@ -1605,13 +1658,13 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>27</v>
@@ -1620,25 +1673,25 @@
         <v>27</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O25" s="3"/>
       <c r="Q25" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>45</v>
@@ -1647,13 +1700,13 @@
         <v>46</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>47</v>
@@ -1670,33 +1723,33 @@
       <c r="K26" s="2"/>
       <c r="O26" s="3"/>
       <c r="Q26" s="1" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>27</v>
@@ -1705,43 +1758,43 @@
         <v>47</v>
       </c>
       <c r="I27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="O27" s="3"/>
       <c r="Q27" s="1" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>47</v>
@@ -1753,7 +1806,7 @@
         <v>113</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1761,189 +1814,13 @@
       <c r="N28" s="2"/>
       <c r="O28" s="3"/>
       <c r="Q28" s="1" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O29" s="3"/>
-      <c r="Q29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30" s="2"/>
-      <c r="O30" s="3"/>
-      <c r="Q30" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="O31" s="3"/>
-      <c r="Q31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="3"/>
-      <c r="Q32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1952,6 +1829,9 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:N16"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="J19:M19"/>
     <mergeCell ref="J20:N20"/>
@@ -1961,9 +1841,6 @@
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="J27:M27"/>
     <mergeCell ref="J28:N28"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:N32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
found a typeo in the sample sheet.
Also reran the sample estimation worksheet with the new naming system
for experiments/batches.  It took rather longer than I expected due to
some confusion on my part.
</commit_message>
<xml_diff>
--- a/sample_sheets/all_samples.xlsx
+++ b/sample_sheets/all_samples.xlsx
@@ -140,7 +140,7 @@
     <t xml:space="preserve">processed_data/count_tables/hpgl0565/hpgl0565_scerevisiae.count.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">Preprocessing/E1/hpgl0565/hpgl0565_scerevisiae.count.xz</t>
+    <t xml:space="preserve">preprocessing/E1/hpgl0565/hpgl0565_scerevisiae.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0566</t>
@@ -682,8 +682,8 @@
   </sheetPr>
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N3" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>